<commit_message>
Add buildHierarchy(). Modify pid-nodes, pid-connections and pid-shapes-libray
</commit_message>
<xml_diff>
--- a/3 Entwicklungsphase/pid-nodes.xlsx
+++ b/3 Entwicklungsphase/pid-nodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Google Drive\TUM\Maschinenwesen B.Sc\Bachelorarbeit\3 Entwicklungsphase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE91693-95E5-4175-9EF4-8B4E88A4B022}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D241B7-B0EC-43F1-9803-DFC7C437F460}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12198" xr2:uid="{35548865-5398-47E6-943D-8DFDE216ADEA}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Control_valve_340_59</t>
   </si>
   <si>
-    <t>Control_valve_340</t>
-  </si>
-  <si>
     <t>Water_supply</t>
   </si>
   <si>
@@ -586,6 +583,9 @@
   </si>
   <si>
     <t>I7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BC155FA-57AA-450D-BD7C-FBC7E34A5435}">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
@@ -1065,31 +1065,31 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -1099,13 +1099,13 @@
     </row>
     <row r="2" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A2" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20">
@@ -1117,16 +1117,16 @@
     </row>
     <row r="3" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="8">
         <v>1</v>
@@ -1137,16 +1137,16 @@
     </row>
     <row r="4" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="8">
         <v>2</v>
@@ -1157,16 +1157,16 @@
     </row>
     <row r="5" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="8">
         <v>3</v>
@@ -1177,16 +1177,16 @@
     </row>
     <row r="6" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" s="12">
         <v>4</v>
@@ -1200,19 +1200,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E7" s="8">
         <v>5</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -1220,41 +1220,41 @@
     </row>
     <row r="8" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E8" s="8">
         <v>5</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" s="12">
         <v>4</v>
@@ -1265,22 +1265,22 @@
     </row>
     <row r="10" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" s="8">
         <v>5</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -1288,26 +1288,26 @@
     </row>
     <row r="11" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" s="8">
         <v>5</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I11" s="10">
         <v>4000</v>
@@ -1315,26 +1315,26 @@
     </row>
     <row r="12" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="8">
         <v>5</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I12" s="10">
         <v>4000</v>
@@ -1342,14 +1342,14 @@
     </row>
     <row r="13" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" s="8">
         <v>5</v>
@@ -1360,14 +1360,14 @@
     </row>
     <row r="14" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E14" s="8">
         <v>5</v>
@@ -1378,16 +1378,16 @@
     </row>
     <row r="15" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="8">
         <v>3</v>
@@ -1398,16 +1398,16 @@
     </row>
     <row r="16" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" s="12">
         <v>4</v>
@@ -1421,19 +1421,19 @@
         <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E17" s="8">
         <v>5</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -1441,41 +1441,41 @@
     </row>
     <row r="18" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E18" s="8">
         <v>5</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A19" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E19" s="12">
         <v>4</v>
@@ -1486,22 +1486,22 @@
     </row>
     <row r="20" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20" s="8">
         <v>5</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
@@ -1509,26 +1509,26 @@
     </row>
     <row r="21" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A21" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E21" s="8">
         <v>5</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I21" s="10">
         <v>1000</v>
@@ -1536,26 +1536,26 @@
     </row>
     <row r="22" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A22" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22" s="8">
         <v>5</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I22" s="10">
         <v>1000</v>
@@ -1563,26 +1563,26 @@
     </row>
     <row r="23" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A23" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E23" s="8">
         <v>5</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I23" s="10">
         <v>1000</v>
@@ -1590,14 +1590,14 @@
     </row>
     <row r="24" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E24" s="8">
         <v>5</v>
@@ -1608,14 +1608,14 @@
     </row>
     <row r="25" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E25" s="8">
         <v>5</v>
@@ -1626,14 +1626,14 @@
     </row>
     <row r="26" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E26" s="8">
         <v>5</v>
@@ -1644,16 +1644,16 @@
     </row>
     <row r="27" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E27" s="12">
         <v>4</v>
@@ -1667,19 +1667,19 @@
         <v>3</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="8">
         <v>5</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -1690,19 +1690,19 @@
         <v>3</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" s="8">
         <v>5</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -1710,16 +1710,16 @@
     </row>
     <row r="30" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E30" s="8">
         <v>3</v>
@@ -1730,16 +1730,16 @@
     </row>
     <row r="31" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" s="12">
         <v>4</v>
@@ -1753,19 +1753,19 @@
         <v>3</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E32" s="8">
         <v>5</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
@@ -1776,19 +1776,19 @@
         <v>3</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E33" s="8">
         <v>5</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
@@ -1799,19 +1799,19 @@
         <v>3</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E34" s="8">
         <v>5</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -1822,19 +1822,19 @@
         <v>3</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E35" s="8">
         <v>5</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
@@ -1845,19 +1845,19 @@
         <v>3</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E36" s="8">
         <v>5</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
@@ -1868,19 +1868,19 @@
         <v>3</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E37" s="8">
         <v>5</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
@@ -1891,19 +1891,19 @@
         <v>3</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E38" s="8">
         <v>5</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
@@ -1914,19 +1914,19 @@
         <v>3</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E39" s="8">
         <v>5</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
@@ -1937,19 +1937,19 @@
         <v>3</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E40" s="8">
         <v>5</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
@@ -1957,26 +1957,26 @@
     </row>
     <row r="41" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E41" s="8">
         <v>5</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G41" s="10"/>
       <c r="H41" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I41" s="10">
         <v>3000</v>
@@ -1987,19 +1987,19 @@
         <v>3</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D42" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="8">
+        <v>5</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="E42" s="8">
-        <v>5</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>48</v>
       </c>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
@@ -2007,21 +2007,21 @@
     </row>
     <row r="43" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A43" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E43" s="8">
         <v>5</v>
       </c>
       <c r="G43" s="10"/>
       <c r="H43" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I43" s="10">
         <v>3000</v>
@@ -2029,16 +2029,16 @@
     </row>
     <row r="44" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E44" s="12">
         <v>4</v>
@@ -2052,19 +2052,19 @@
         <v>3</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E45" s="8">
         <v>5</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G45" s="10"/>
       <c r="H45" s="10"/>
@@ -2075,19 +2075,19 @@
         <v>3</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E46" s="8">
         <v>5</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
@@ -2098,19 +2098,19 @@
         <v>3</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E47" s="9">
         <v>5</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -2121,19 +2121,19 @@
         <v>3</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E48" s="9">
         <v>5</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -2144,19 +2144,19 @@
         <v>3</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E49" s="9">
         <v>5</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -2167,19 +2167,19 @@
         <v>3</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E50" s="9">
         <v>5</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -2187,41 +2187,41 @@
     </row>
     <row r="51" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A51" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E51" s="9">
         <v>5</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
     </row>
     <row r="52" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A52" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E52" s="9">
         <v>3</v>
@@ -2233,16 +2233,16 @@
     </row>
     <row r="53" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E53" s="15">
         <v>4</v>
@@ -2257,19 +2257,19 @@
         <v>3</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E54" s="9">
         <v>5</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -2277,16 +2277,16 @@
     </row>
     <row r="55" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A55" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E55" s="12">
         <v>4</v>
@@ -2300,19 +2300,19 @@
         <v>3</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E56" s="8">
         <v>5</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
@@ -2320,26 +2320,26 @@
     </row>
     <row r="57" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A57" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E57" s="8">
         <v>5</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G57" s="10"/>
       <c r="H57" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I57" s="10">
         <v>2000</v>
@@ -2347,26 +2347,26 @@
     </row>
     <row r="58" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A58" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E58" s="8">
         <v>5</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G58" s="10"/>
       <c r="H58" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I58" s="10">
         <v>2000</v>
@@ -2374,21 +2374,21 @@
     </row>
     <row r="59" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A59" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E59" s="8">
         <v>5</v>
       </c>
       <c r="G59" s="10"/>
       <c r="H59" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I59" s="10">
         <v>2000</v>
@@ -2396,16 +2396,16 @@
     </row>
     <row r="60" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E60" s="12">
         <v>4</v>
@@ -2419,10 +2419,10 @@
         <v>3</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>9</v>
+        <v>186</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>1</v>
@@ -2442,7 +2442,7 @@
         <v>3</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>7</v>
@@ -2465,7 +2465,7 @@
         <v>3</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>5</v>
@@ -2488,7 +2488,7 @@
         <v>3</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>2</v>

</xml_diff>